<commit_message>
Hcl tags added. Removed null values to avoid optimizer fail. Handled optimizer fail cases, where current allocation is added
</commit_message>
<xml_diff>
--- a/data/Data Request Detailed_19062025.xlsx
+++ b/data/Data Request Detailed_19062025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Anshul_Agarwal/Library/CloudStorage/Box-Box/DCM/99 Working folders/14 Anshul/Margin Maximizer/integrated_margin_maximizer/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{845B9C45-61E2-D241-9C17-8765649D31D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F652DA00-0E36-294A-8C6C-71C239163D74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="860" windowWidth="25840" windowHeight="17800" activeTab="3" xr2:uid="{B49C1CC5-7DB3-794A-B170-F3399E5F60B1}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1623" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1624" uniqueCount="391">
   <si>
     <t>Type</t>
   </si>
@@ -5812,18 +5812,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:A30"/>
+    <mergeCell ref="B2:B30"/>
+    <mergeCell ref="B31:B51"/>
+    <mergeCell ref="A31:A51"/>
+    <mergeCell ref="A52:A75"/>
+    <mergeCell ref="B52:B75"/>
     <mergeCell ref="A76:A86"/>
     <mergeCell ref="B76:B86"/>
     <mergeCell ref="A87:A97"/>
     <mergeCell ref="B87:B97"/>
     <mergeCell ref="A98:A110"/>
     <mergeCell ref="B98:B110"/>
-    <mergeCell ref="A2:A30"/>
-    <mergeCell ref="B2:B30"/>
-    <mergeCell ref="B31:B51"/>
-    <mergeCell ref="A31:A51"/>
-    <mergeCell ref="A52:A75"/>
-    <mergeCell ref="B52:B75"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -11013,8 +11013,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC5ED671-0947-D741-A9ED-72DD6B28D57E}">
   <dimension ref="A1:O126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="132" workbookViewId="0">
-      <selection activeCell="L67" sqref="L67:O73"/>
+    <sheetView tabSelected="1" topLeftCell="F4" zoomScale="118" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21:O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11412,6 +11412,9 @@
       </c>
       <c r="N10" t="s">
         <v>218</v>
+      </c>
+      <c r="O10" t="s">
+        <v>380</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">

</xml_diff>